<commit_message>
Main changes and the scrapped code lines.
Fixing bugs. Will clean it.
</commit_message>
<xml_diff>
--- a/src/test/resources/test-data/Parameters for VES.xlsx
+++ b/src/test/resources/test-data/Parameters for VES.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23127"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23530"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\salturk\IdeaProjects\AutomationFramework\src\test\resources\test-data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5859F7C8-2F02-433A-8C66-B50720386588}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{78850C84-E89E-4A44-B293-5429F5CD6936}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16896" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-30828" yWindow="-108" windowWidth="30936" windowHeight="16896" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="32">
   <si>
     <t>TV</t>
   </si>
@@ -86,21 +86,12 @@
     <t>Phone</t>
   </si>
   <si>
-    <t>BatteryBackup</t>
-  </si>
-  <si>
     <t>Replacement Power Cord DVR</t>
   </si>
   <si>
-    <t>Replacement RemoteControl DVR</t>
-  </si>
-  <si>
     <t>Replacement Power Cord STB</t>
   </si>
   <si>
-    <t>Replacement RemoteControl STB</t>
-  </si>
-  <si>
     <t>Unreturned DVR</t>
   </si>
   <si>
@@ -836,6 +827,15 @@
   </si>
   <si>
     <t>r</t>
+  </si>
+  <si>
+    <t>Replacement Remote Control DVR</t>
+  </si>
+  <si>
+    <t>Replacement Remote Control STB</t>
+  </si>
+  <si>
+    <t>Battery Backup</t>
   </si>
 </sst>
 </file>
@@ -1203,43 +1203,44 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AF42"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="U1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3:AF42"/>
+    <sheetView tabSelected="1" topLeftCell="G1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="Q2" sqref="Q2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="4" customWidth="1"/>
-    <col min="2" max="2" width="5.21875" customWidth="1"/>
-    <col min="3" max="3" width="4.33203125" customWidth="1"/>
-    <col min="4" max="4" width="26" customWidth="1"/>
-    <col min="5" max="5" width="28.77734375" customWidth="1"/>
-    <col min="6" max="6" width="14.5546875" customWidth="1"/>
-    <col min="7" max="7" width="4.6640625" customWidth="1"/>
-    <col min="8" max="8" width="25.77734375" customWidth="1"/>
-    <col min="9" max="9" width="29.33203125" customWidth="1"/>
-    <col min="10" max="10" width="14.44140625" customWidth="1"/>
-    <col min="11" max="11" width="7.33203125" customWidth="1"/>
-    <col min="12" max="12" width="9.77734375" customWidth="1"/>
-    <col min="13" max="13" width="4.77734375" customWidth="1"/>
-    <col min="14" max="14" width="7.88671875" customWidth="1"/>
-    <col min="16" max="16" width="4.33203125" customWidth="1"/>
-    <col min="17" max="17" width="7.44140625" customWidth="1"/>
-    <col min="18" max="18" width="6.44140625" customWidth="1"/>
-    <col min="19" max="19" width="7" customWidth="1"/>
-    <col min="20" max="20" width="15.33203125" customWidth="1"/>
-    <col min="21" max="21" width="16.88671875" customWidth="1"/>
-    <col min="22" max="22" width="15" customWidth="1"/>
-    <col min="23" max="23" width="16.77734375" customWidth="1"/>
-    <col min="24" max="24" width="24.6640625" customWidth="1"/>
-    <col min="25" max="25" width="25.5546875" customWidth="1"/>
-    <col min="26" max="26" width="17.33203125" customWidth="1"/>
-    <col min="27" max="27" width="23.6640625" customWidth="1"/>
+    <col min="1" max="1" width="3.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="4.6640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="28.109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="32" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="15.5546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="4.109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="27.5546875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="31.44140625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="15" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="7.5546875" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="10.44140625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="5.33203125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="8.6640625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="10" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="4.88671875" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="6.5546875" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="7" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="16.6640625" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="18" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="15.6640625" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="18" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="25.88671875" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="26.88671875" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="18.5546875" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="25.6640625" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="26.6640625" bestFit="1" customWidth="1"/>
     <col min="28" max="28" width="25" customWidth="1"/>
     <col min="29" max="29" width="19" customWidth="1"/>
-    <col min="30" max="30" width="13.77734375" customWidth="1"/>
+    <col min="30" max="30" width="14.33203125" bestFit="1" customWidth="1"/>
     <col min="31" max="31" width="13.109375" customWidth="1"/>
-    <col min="32" max="32" width="1.77734375" customWidth="1"/>
+    <col min="32" max="32" width="1.6640625" customWidth="1"/>
     <col min="33" max="33" width="13.109375" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1248,31 +1249,31 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>1</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="E1" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="F1" s="1" t="s">
         <v>19</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>22</v>
       </c>
       <c r="G1" s="1" t="s">
         <v>2</v>
       </c>
       <c r="H1" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="J1" s="1" t="s">
         <v>20</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>23</v>
       </c>
       <c r="K1" s="1" t="s">
         <v>3</v>
@@ -1293,7 +1294,7 @@
         <v>8</v>
       </c>
       <c r="Q1" s="1" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="R1" s="1" t="s">
         <v>9</v>
@@ -1311,19 +1312,19 @@
         <v>13</v>
       </c>
       <c r="W1" s="1" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="X1" s="1" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="Y1" s="1" t="s">
         <v>14</v>
       </c>
       <c r="Z1" s="1" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="AA1" s="1" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="AB1" s="1" t="s">
         <v>15</v>
@@ -1332,96 +1333,96 @@
         <v>16</v>
       </c>
       <c r="AD1" s="2" t="s">
-        <v>17</v>
+        <v>31</v>
       </c>
     </row>
     <row r="2" spans="1:32" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="F2" s="3" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="G2" s="3" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="H2" s="3" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="I2" s="3" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="J2" s="3" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="K2" s="3" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="L2" s="3" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="M2" s="3" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="N2" s="3" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="O2" s="3" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="P2" s="3" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="Q2" s="3" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="R2" s="3" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="S2" s="3" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="T2" s="3" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="U2" s="3" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="V2" s="3" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="W2" s="3" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="X2" s="3" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="Y2" s="3" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="Z2" s="3" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="AA2" s="3" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="AB2" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="AC2" s="3" t="s">
-        <v>31</v>
+        <v>28</v>
+      </c>
+      <c r="AC2" s="3">
+        <v>0</v>
       </c>
       <c r="AD2" s="3">
         <v>0</v>
@@ -1429,7 +1430,7 @@
     </row>
     <row r="3" spans="1:32" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="5" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="B3" s="5"/>
       <c r="C3" s="5"/>

</xml_diff>